<commit_message>
seguimiento del servicio social
</commit_message>
<xml_diff>
--- a/Seguimiento Servicio Social.xlsx
+++ b/Seguimiento Servicio Social.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="7740"/>
+    <workbookView xWindow="0" yWindow="1200" windowWidth="20490" windowHeight="7740"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Semana</t>
   </si>
@@ -81,6 +81,18 @@
   </si>
   <si>
     <t>Mejoras a la pagina e investigacion de nuevas caracteristicas</t>
+  </si>
+  <si>
+    <t>Fue semana de examenes, y no tube mucho tiempo</t>
+  </si>
+  <si>
+    <t>4 Octubre - 11 Octubre</t>
+  </si>
+  <si>
+    <t>11 Octubre - 18- Octubre</t>
+  </si>
+  <si>
+    <t>18 Octubre - 25 Octubre</t>
   </si>
 </sst>
 </file>
@@ -603,7 +615,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
@@ -708,9 +720,13 @@
       <c r="B9" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="4">
+        <v>0</v>
+      </c>
       <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="E9" s="7" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B10" s="4" t="s">
@@ -721,19 +737,25 @@
       <c r="E10" s="7"/>
     </row>
     <row r="11" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B11" s="4"/>
+      <c r="B11" s="4" t="s">
+        <v>20</v>
+      </c>
       <c r="C11" s="4"/>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
     </row>
     <row r="12" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B12" s="4"/>
+      <c r="B12" s="4" t="s">
+        <v>21</v>
+      </c>
       <c r="C12" s="4"/>
       <c r="D12" s="7"/>
       <c r="E12" s="7"/>
     </row>
     <row r="13" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
+      <c r="B13" s="4" t="s">
+        <v>22</v>
+      </c>
       <c r="C13" s="4"/>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>

</xml_diff>